<commit_message>
fix: added internal data aggregation to handle slicer granularity. chore: updated example dataset with category columns
</commit_message>
<xml_diff>
--- a/dataset_Example.xlsx
+++ b/dataset_Example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\002. MANUEL VASQUEZ\PowerBI\01_Sankey_Diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\002. MANUEL VASQUEZ\PowerBI\Sankey_Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68330C37-DC9C-4276-BAD1-4CB4FCE1DA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01F57F4-7028-4D6D-BC90-34D7D6C696CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65DD97F2-0BE6-4DD6-B425-9CB9AA1C940C}"/>
   </bookViews>
@@ -185,6 +185,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2FDB51D1-4478-4ABE-A598-4CE09386341C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">manuelvasquezab:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Podemos adicionar diferentes columnas para el filtrado mediante un slicer en Power BI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{A8FA2DC6-C8B6-40B7-B67B-B894FA9B1CE2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">manuelvasquezab:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Podemos adicionar diferentes columnas para el filtrado mediante un slicer en Power BI</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -210,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="26">
   <si>
     <t>Source</t>
   </si>
@@ -264,6 +312,30 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Categoría Nivel 1</t>
+  </si>
+  <si>
+    <t>Categoría Nivel 2</t>
+  </si>
+  <si>
+    <t>Categoría A</t>
+  </si>
+  <si>
+    <t>Categoría B</t>
+  </si>
+  <si>
+    <t>Subcategoría A</t>
+  </si>
+  <si>
+    <t>Subcategoría B</t>
+  </si>
+  <si>
+    <t>Subcategoría C</t>
+  </si>
+  <si>
+    <t>Subcategoría D</t>
   </si>
 </sst>
 </file>
@@ -400,20 +472,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8096D2A5-8168-43F2-B69E-609B2E9B5A23}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,9 +835,11 @@
     <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -783,8 +858,14 @@
       <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -803,8 +884,14 @@
       <c r="F2" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -823,8 +910,14 @@
       <c r="F3" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -843,8 +936,14 @@
       <c r="F4" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -863,8 +962,14 @@
       <c r="F5" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -883,8 +988,14 @@
       <c r="F6" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>3</v>
       </c>
@@ -903,8 +1014,14 @@
       <c r="F7" s="12">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -923,8 +1040,14 @@
       <c r="F8" s="9">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>4</v>
       </c>
@@ -943,8 +1066,14 @@
       <c r="F9" s="12">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -963,8 +1092,14 @@
       <c r="F10" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>4</v>
       </c>
@@ -983,8 +1118,14 @@
       <c r="F11" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1002,6 +1143,870 @@
       </c>
       <c r="F12" s="3">
         <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>26032163.75</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="11">
+        <v>4593911.2500000009</v>
+      </c>
+      <c r="F14" s="12">
+        <v>2</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>28727258.350000001</v>
+      </c>
+      <c r="F15" s="9">
+        <v>3</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>2</v>
+      </c>
+      <c r="B16" s="11">
+        <v>3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11">
+        <v>1898816.6500000001</v>
+      </c>
+      <c r="F16" s="12">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>3</v>
+      </c>
+      <c r="B17" s="8">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>27930980.400000002</v>
+      </c>
+      <c r="F17" s="9">
+        <v>5</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>3</v>
+      </c>
+      <c r="B18" s="11">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="11">
+        <v>551269.35000000009</v>
+      </c>
+      <c r="F18" s="12">
+        <v>6</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>3</v>
+      </c>
+      <c r="B19" s="8">
+        <v>4</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="8">
+        <v>245008.6</v>
+      </c>
+      <c r="F19" s="9">
+        <v>7</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>4</v>
+      </c>
+      <c r="B20" s="11">
+        <v>5</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11">
+        <v>26736563.475000001</v>
+      </c>
+      <c r="F20" s="12">
+        <v>8</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>4</v>
+      </c>
+      <c r="B21" s="8">
+        <v>5</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="8">
+        <v>612521.5</v>
+      </c>
+      <c r="F21" s="9">
+        <v>9</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>4</v>
+      </c>
+      <c r="B22" s="11">
+        <v>5</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="11">
+        <v>520643.27500000002</v>
+      </c>
+      <c r="F22" s="12">
+        <v>10</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2">
+        <v>61252.15</v>
+      </c>
+      <c r="F23" s="3">
+        <v>11</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>1</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="8">
+        <v>26032163.75</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="11">
+        <v>4593911.2500000009</v>
+      </c>
+      <c r="F25" s="12">
+        <v>2</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8">
+        <v>3</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="8">
+        <v>28727258.350000001</v>
+      </c>
+      <c r="F26" s="9">
+        <v>3</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>2</v>
+      </c>
+      <c r="B27" s="11">
+        <v>3</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11">
+        <v>1898816.6500000001</v>
+      </c>
+      <c r="F27" s="12">
+        <v>4</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>3</v>
+      </c>
+      <c r="B28" s="8">
+        <v>4</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="8">
+        <v>27930980.400000002</v>
+      </c>
+      <c r="F28" s="9">
+        <v>5</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>3</v>
+      </c>
+      <c r="B29" s="11">
+        <v>4</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="11">
+        <v>551269.35000000009</v>
+      </c>
+      <c r="F29" s="12">
+        <v>6</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>3</v>
+      </c>
+      <c r="B30" s="8">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="8">
+        <v>245008.6</v>
+      </c>
+      <c r="F30" s="9">
+        <v>7</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
+        <v>4</v>
+      </c>
+      <c r="B31" s="11">
+        <v>5</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="11">
+        <v>26736563.475000001</v>
+      </c>
+      <c r="F31" s="12">
+        <v>8</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>4</v>
+      </c>
+      <c r="B32" s="8">
+        <v>5</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="8">
+        <v>612521.5</v>
+      </c>
+      <c r="F32" s="9">
+        <v>9</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
+        <v>4</v>
+      </c>
+      <c r="B33" s="11">
+        <v>5</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="11">
+        <v>520643.27500000002</v>
+      </c>
+      <c r="F33" s="12">
+        <v>10</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2">
+        <v>61252.15</v>
+      </c>
+      <c r="F34" s="3">
+        <v>11</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>1</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="8">
+        <v>26032163.75</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
+        <v>1</v>
+      </c>
+      <c r="B36" s="11">
+        <v>2</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="11">
+        <v>4593911.2500000009</v>
+      </c>
+      <c r="F36" s="12">
+        <v>2</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>2</v>
+      </c>
+      <c r="B37" s="8">
+        <v>3</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="8">
+        <v>28727258.350000001</v>
+      </c>
+      <c r="F37" s="9">
+        <v>3</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
+        <v>2</v>
+      </c>
+      <c r="B38" s="11">
+        <v>3</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="11">
+        <v>1898816.6500000001</v>
+      </c>
+      <c r="F38" s="12">
+        <v>4</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>3</v>
+      </c>
+      <c r="B39" s="8">
+        <v>4</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="8">
+        <v>27930980.400000002</v>
+      </c>
+      <c r="F39" s="9">
+        <v>5</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="10">
+        <v>3</v>
+      </c>
+      <c r="B40" s="11">
+        <v>4</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="11">
+        <v>551269.35000000009</v>
+      </c>
+      <c r="F40" s="12">
+        <v>6</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>3</v>
+      </c>
+      <c r="B41" s="8">
+        <v>4</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="8">
+        <v>245008.6</v>
+      </c>
+      <c r="F41" s="9">
+        <v>7</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11">
+        <v>5</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="11">
+        <v>26736563.475000001</v>
+      </c>
+      <c r="F42" s="12">
+        <v>8</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>4</v>
+      </c>
+      <c r="B43" s="8">
+        <v>5</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="8">
+        <v>612521.5</v>
+      </c>
+      <c r="F43" s="9">
+        <v>9</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="10">
+        <v>4</v>
+      </c>
+      <c r="B44" s="11">
+        <v>5</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="11">
+        <v>520643.27500000002</v>
+      </c>
+      <c r="F44" s="12">
+        <v>10</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2">
+        <v>5</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="2">
+        <v>61252.15</v>
+      </c>
+      <c r="F45" s="3">
+        <v>11</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>